<commit_message>
More pandas analysis with plots in notebook
</commit_message>
<xml_diff>
--- a/Iliad_battles.xlsx
+++ b/Iliad_battles.xlsx
@@ -1471,7 +1471,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1508,12 +1508,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1535,7 +1529,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1570,9 +1564,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1879,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H286"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A49" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -5055,10 +5046,10 @@
       </c>
     </row>
     <row r="123" spans="1:8">
-      <c r="A123" s="15" t="s">
+      <c r="A123" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="14" t="s">
         <v>235</v>
       </c>
       <c r="C123" s="4" t="s">
@@ -5364,7 +5355,7 @@
       </c>
     </row>
     <row r="135" spans="1:8">
-      <c r="A135" s="14" t="s">
+      <c r="A135" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B135" s="9" t="s">
@@ -6679,7 +6670,7 @@
       <c r="G185" s="6">
         <v>16.114000000000001</v>
       </c>
-      <c r="H185" s="16" t="s">
+      <c r="H185" s="15" t="s">
         <v>351</v>
       </c>
     </row>
@@ -8732,7 +8723,7 @@
       <c r="A273" s="1"/>
     </row>
     <row r="274" spans="1:1">
-      <c r="A274" s="13"/>
+      <c r="A274" s="1"/>
     </row>
     <row r="275" spans="1:1">
       <c r="A275" s="1"/>

</xml_diff>

<commit_message>
Further small changes to notebook (clean-up and editing)
</commit_message>
<xml_diff>
--- a/Iliad_battles.xlsx
+++ b/Iliad_battles.xlsx
@@ -1203,9 +1203,6 @@
     <t>Sthenelaos killed stone to the neck (16.586-7)</t>
   </si>
   <si>
-    <t>Glaukos son of Hippolochos</t>
-  </si>
-  <si>
     <t>Bathykles, son of Chalkon</t>
   </si>
   <si>
@@ -1462,6 +1459,9 @@
   </si>
   <si>
     <t>Thoas the Aitolian</t>
+  </si>
+  <si>
+    <t>Glaukos, son of Hippolochos</t>
   </si>
 </sst>
 </file>
@@ -1870,8 +1870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A49" sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A213" sqref="A213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="8" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>25</v>
@@ -7352,10 +7352,10 @@
     </row>
     <row r="212" spans="1:8">
       <c r="A212" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="B212" s="9" t="s">
         <v>395</v>
-      </c>
-      <c r="B212" s="9" t="s">
-        <v>396</v>
       </c>
       <c r="C212" s="4" t="s">
         <v>3</v>
@@ -7373,7 +7373,7 @@
         <v>16.597000000000001</v>
       </c>
       <c r="H212" s="9" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="213" spans="1:8">
@@ -7381,7 +7381,7 @@
         <v>47</v>
       </c>
       <c r="B213" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C213" s="4" t="s">
         <v>2</v>
@@ -7399,7 +7399,7 @@
         <v>16.603000000000002</v>
       </c>
       <c r="H213" s="9" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="214" spans="1:8">
@@ -7425,7 +7425,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H214" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="215" spans="1:8">
@@ -7451,7 +7451,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H215" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="216" spans="1:8">
@@ -7459,7 +7459,7 @@
         <v>352</v>
       </c>
       <c r="B216" s="9" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C216" s="4" t="s">
         <v>2</v>
@@ -7477,7 +7477,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H216" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="217" spans="1:8">
@@ -7485,7 +7485,7 @@
         <v>352</v>
       </c>
       <c r="B217" s="9" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C217" s="4" t="s">
         <v>2</v>
@@ -7503,7 +7503,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H217" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="218" spans="1:8">
@@ -7511,7 +7511,7 @@
         <v>352</v>
       </c>
       <c r="B218" s="9" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C218" s="4" t="s">
         <v>2</v>
@@ -7529,7 +7529,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H218" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="219" spans="1:8">
@@ -7555,7 +7555,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H219" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="220" spans="1:8">
@@ -7563,7 +7563,7 @@
         <v>352</v>
       </c>
       <c r="B220" s="9" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C220" s="4" t="s">
         <v>2</v>
@@ -7581,7 +7581,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H220" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="221" spans="1:8">
@@ -7589,7 +7589,7 @@
         <v>352</v>
       </c>
       <c r="B221" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C221" s="4" t="s">
         <v>2</v>
@@ -7607,7 +7607,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H221" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="222" spans="1:8">
@@ -7633,7 +7633,7 @@
         <v>16.693000000000001</v>
       </c>
       <c r="H222" s="9" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="223" spans="1:8">
@@ -7641,7 +7641,7 @@
         <v>352</v>
       </c>
       <c r="B223" s="9" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C223" s="4" t="s">
         <v>2</v>
@@ -7659,7 +7659,7 @@
         <v>16.733000000000001</v>
       </c>
       <c r="H223" s="9" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="224" spans="1:8" ht="27" customHeight="1">
@@ -7667,7 +7667,7 @@
         <v>352</v>
       </c>
       <c r="B224" s="9" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C224" s="4" t="s">
         <v>2</v>
@@ -7685,7 +7685,7 @@
         <v>16.783000000000001</v>
       </c>
       <c r="H224" s="9" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -7693,7 +7693,7 @@
         <v>44</v>
       </c>
       <c r="B225" s="9" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C225" s="4" t="s">
         <v>2</v>
@@ -7711,7 +7711,7 @@
         <v>17.042999999999999</v>
       </c>
       <c r="H225" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -7719,7 +7719,7 @@
         <v>44</v>
       </c>
       <c r="B226" s="9" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C226" s="4" t="s">
         <v>2</v>
@@ -7737,7 +7737,7 @@
         <v>17.288</v>
       </c>
       <c r="H226" s="9" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="227" spans="1:8" ht="25.5">
@@ -7745,7 +7745,7 @@
         <v>88</v>
       </c>
       <c r="B227" s="9" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C227" s="4" t="s">
         <v>3</v>
@@ -7763,7 +7763,7 @@
         <v>17.303999999999998</v>
       </c>
       <c r="H227" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -7771,7 +7771,7 @@
         <v>14</v>
       </c>
       <c r="B228" s="9" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>2</v>
@@ -7789,7 +7789,7 @@
         <v>17.312000000000001</v>
       </c>
       <c r="H228" s="9" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -7797,7 +7797,7 @@
         <v>72</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>3</v>
@@ -7815,15 +7815,15 @@
         <v>17.344000000000001</v>
       </c>
       <c r="H229" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="B230" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="B230" s="8" t="s">
-        <v>421</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>2</v>
@@ -7841,15 +7841,15 @@
         <v>17.346</v>
       </c>
       <c r="H230" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="10" t="s">
+        <v>422</v>
+      </c>
+      <c r="B231" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="B231" s="8" t="s">
-        <v>424</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>2</v>
@@ -7867,7 +7867,7 @@
         <v>17.515000000000001</v>
       </c>
       <c r="H231" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="232" spans="1:8">
@@ -7875,7 +7875,7 @@
         <v>44</v>
       </c>
       <c r="B232" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>2</v>
@@ -7893,7 +7893,7 @@
         <v>17.574999999999999</v>
       </c>
       <c r="H232" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="233" spans="1:8">
@@ -7919,7 +7919,7 @@
         <v>17.597000000000001</v>
       </c>
       <c r="H233" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="234" spans="1:8">
@@ -7927,7 +7927,7 @@
         <v>88</v>
       </c>
       <c r="B234" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>3</v>
@@ -7945,7 +7945,7 @@
         <v>17.600999999999999</v>
       </c>
       <c r="H234" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="235" spans="1:8">
@@ -7953,7 +7953,7 @@
         <v>88</v>
       </c>
       <c r="B235" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C235" s="4" t="s">
         <v>3</v>
@@ -7971,12 +7971,12 @@
         <v>17.611000000000001</v>
       </c>
       <c r="H235" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="236" spans="1:8" ht="25.5">
       <c r="A236" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B236" s="9" t="s">
         <v>72</v>
@@ -7994,15 +7994,15 @@
         <v>20.318000000000001</v>
       </c>
       <c r="H236" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="237" spans="1:8">
       <c r="A237" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C237" s="4" t="s">
         <v>2</v>
@@ -8020,15 +8020,15 @@
         <v>20.381</v>
       </c>
       <c r="H237" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="238" spans="1:8">
       <c r="A238" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C238" s="4" t="s">
         <v>2</v>
@@ -8046,15 +8046,15 @@
         <v>20.395</v>
       </c>
       <c r="H238" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B239" s="9" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C239" s="4" t="s">
         <v>2</v>
@@ -8072,15 +8072,15 @@
         <v>20.401</v>
       </c>
       <c r="H239" s="9" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="240" spans="1:8">
       <c r="A240" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B240" s="9" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C240" s="4" t="s">
         <v>2</v>
@@ -8098,12 +8098,12 @@
         <v>20.407</v>
       </c>
       <c r="H240" s="9" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="241" spans="1:8">
       <c r="A241" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B241" s="9" t="s">
         <v>88</v>
@@ -8121,15 +8121,15 @@
         <v>20.437999999999999</v>
       </c>
       <c r="H241" s="9" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="242" spans="1:8">
       <c r="A242" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B242" s="9" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C242" s="4" t="s">
         <v>2</v>
@@ -8147,15 +8147,15 @@
         <v>20.454999999999998</v>
       </c>
       <c r="H242" s="9" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="243" spans="1:8">
       <c r="A243" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B243" s="9" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C243" s="4" t="s">
         <v>2</v>
@@ -8173,15 +8173,15 @@
         <v>20.457000000000001</v>
       </c>
       <c r="H243" s="9" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="244" spans="1:8">
       <c r="A244" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B244" s="9" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C244" s="4" t="s">
         <v>2</v>
@@ -8199,15 +8199,15 @@
         <v>20.465</v>
       </c>
       <c r="H244" s="9" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="245" spans="1:8">
       <c r="A245" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B245" s="9" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C245" s="4" t="s">
         <v>2</v>
@@ -8225,15 +8225,15 @@
         <v>20.472000000000001</v>
       </c>
       <c r="H245" s="9" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="246" spans="1:8">
       <c r="A246" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B246" s="9" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C246" s="4" t="s">
         <v>2</v>
@@ -8251,15 +8251,15 @@
         <v>20.474</v>
       </c>
       <c r="H246" s="9" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="247" spans="1:8">
       <c r="A247" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B247" s="9" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C247" s="4" t="s">
         <v>2</v>
@@ -8277,15 +8277,15 @@
         <v>20.477</v>
       </c>
       <c r="H247" s="9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="248" spans="1:8">
       <c r="A248" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B248" s="9" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C248" s="4" t="s">
         <v>2</v>
@@ -8303,15 +8303,15 @@
         <v>20.484000000000002</v>
       </c>
       <c r="H248" s="9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="249" spans="1:8">
       <c r="A249" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B249" s="9" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C249" s="4" t="s">
         <v>2</v>
@@ -8329,15 +8329,15 @@
         <v>20.486999999999998</v>
       </c>
       <c r="H249" s="9" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="250" spans="1:8">
       <c r="A250" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B250" s="9" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C250" s="4" t="s">
         <v>2</v>
@@ -8355,15 +8355,15 @@
         <v>21.114000000000001</v>
       </c>
       <c r="H250" s="9" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="251" spans="1:8">
       <c r="A251" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B251" s="9" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C251" s="4" t="s">
         <v>2</v>
@@ -8381,15 +8381,15 @@
         <v>21.178999999999998</v>
       </c>
       <c r="H251" s="9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="252" spans="1:8">
       <c r="A252" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B252" s="9" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C252" s="4" t="s">
         <v>2</v>
@@ -8407,15 +8407,15 @@
         <v>21.209</v>
       </c>
       <c r="H252" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="253" spans="1:8">
       <c r="A253" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B253" s="9" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C253" s="4" t="s">
         <v>2</v>
@@ -8433,15 +8433,15 @@
         <v>21.209</v>
       </c>
       <c r="H253" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="254" spans="1:8">
       <c r="A254" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B254" s="9" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C254" s="4" t="s">
         <v>2</v>
@@ -8459,15 +8459,15 @@
         <v>21.209</v>
       </c>
       <c r="H254" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="255" spans="1:8">
       <c r="A255" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B255" s="9" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C255" s="4" t="s">
         <v>2</v>
@@ -8485,15 +8485,15 @@
         <v>21.209</v>
       </c>
       <c r="H255" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="256" spans="1:8">
       <c r="A256" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B256" s="9" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C256" s="4" t="s">
         <v>2</v>
@@ -8511,15 +8511,15 @@
         <v>21.209</v>
       </c>
       <c r="H256" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="257" spans="1:8">
       <c r="A257" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B257" s="9" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C257" s="4" t="s">
         <v>2</v>
@@ -8537,12 +8537,12 @@
         <v>21.209</v>
       </c>
       <c r="H257" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="258" spans="1:8">
       <c r="A258" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B258" s="9" t="s">
         <v>161</v>
@@ -8563,15 +8563,15 @@
         <v>21.209</v>
       </c>
       <c r="H258" s="9" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="259" spans="1:8" ht="25.5">
       <c r="A259" s="9" t="s">
+        <v>469</v>
+      </c>
+      <c r="B259" s="9" t="s">
         <v>470</v>
-      </c>
-      <c r="B259" s="9" t="s">
-        <v>471</v>
       </c>
       <c r="C259" s="4" t="s">
         <v>117</v>
@@ -8586,12 +8586,12 @@
         <v>21.341999999999999</v>
       </c>
       <c r="H259" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="260" spans="1:8">
       <c r="A260" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B260" s="9" t="s">
         <v>113</v>
@@ -8612,12 +8612,12 @@
         <v>21.402000000000001</v>
       </c>
       <c r="H260" s="9" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="261" spans="1:8">
       <c r="A261" s="10" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B261" s="9" t="s">
         <v>74</v>
@@ -8638,15 +8638,15 @@
         <v>21.422999999999998</v>
       </c>
       <c r="H261" s="9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="262" spans="1:8">
       <c r="A262" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="B262" s="9" t="s">
         <v>476</v>
-      </c>
-      <c r="B262" s="9" t="s">
-        <v>477</v>
       </c>
       <c r="C262" s="4" t="s">
         <v>117</v>
@@ -8664,12 +8664,12 @@
         <v>21.489000000000001</v>
       </c>
       <c r="H262" s="9" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="263" spans="1:8" ht="25.5">
       <c r="A263" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B263" s="9" t="s">
         <v>13</v>
@@ -8687,12 +8687,12 @@
         <v>21.59</v>
       </c>
       <c r="H263" s="9" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="264" spans="1:8" ht="27" customHeight="1">
       <c r="A264" s="10" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B264" s="9" t="s">
         <v>88</v>
@@ -8713,7 +8713,7 @@
         <v>22.306000000000001</v>
       </c>
       <c r="H264" s="9" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="272" spans="1:8">

</xml_diff>